<commit_message>
Reformat questions for adding labels and images, plus creation of functional xlsx upload
</commit_message>
<xml_diff>
--- a/extras/example.xlsx
+++ b/extras/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TFG_repos\tfg-api\extras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203434C4-DFD4-4C3C-800F-2A1C1F286D28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE66288-D080-4311-BA9F-0642FF9136F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13860" yWindow="2310" windowWidth="23445" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14595" yWindow="2280" windowWidth="23445" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="questions" sheetId="1" r:id="rId1"/>
@@ -45,9 +45,6 @@
     <t>respuesta 1;respuesta 2;respuesta 3;respuesta 4</t>
   </si>
   <si>
-    <t>2;3</t>
-  </si>
-  <si>
     <t>test;microbiology;computer science</t>
   </si>
   <si>
@@ -61,6 +58,9 @@
   </si>
   <si>
     <t>https://myimage.png</t>
+  </si>
+  <si>
+    <t>2; (O respuesta múltiple, 2;4;)</t>
   </si>
 </sst>
 </file>
@@ -113,10 +113,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -398,63 +400,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>10</v>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F3" s="2"/>
+      <c r="C3" s="4"/>
+      <c r="F3" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>